<commit_message>
clean cells copy and paste pev
</commit_message>
<xml_diff>
--- a/auto.xlsx
+++ b/auto.xlsx
@@ -8,6 +8,8 @@
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="created_sheet_20230830_140614" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="created_sheet_20230901_143340" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="created_sheet_20230901_144622" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -747,4 +749,314 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test 1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test 2</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test 3</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test 4</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>test 1</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test 2</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test 3</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>test 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" t="n">
+        <v>14</v>
+      </c>
+      <c r="H2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>th</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B3" t="n">
+        <v>14</v>
+      </c>
+      <c r="D3" t="n">
+        <v>28</v>
+      </c>
+      <c r="H3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>sasa</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>25</v>
+      </c>
+      <c r="B4" t="n">
+        <v>69</v>
+      </c>
+      <c r="D4" t="n">
+        <v>39</v>
+      </c>
+      <c r="H4" t="n">
+        <v>69</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>asasa</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>35</v>
+      </c>
+      <c r="B5" t="n">
+        <v>74</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" t="n">
+        <v>74</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>asfd</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test 1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>test 2</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>test 3</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>test 4</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>test 1</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>test 2</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>test 3</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>test 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" t="n">
+        <v>14</v>
+      </c>
+      <c r="H2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>th</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B3" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" t="n">
+        <v>28</v>
+      </c>
+      <c r="H3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>sasa</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>25</v>
+      </c>
+      <c r="B4" t="n">
+        <v>69</v>
+      </c>
+      <c r="C4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>39</v>
+      </c>
+      <c r="H4" t="n">
+        <v>69</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>asasa</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>35</v>
+      </c>
+      <c r="B5" t="n">
+        <v>74</v>
+      </c>
+      <c r="C5" t="n">
+        <v>35</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" t="n">
+        <v>74</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>asfd</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>